<commit_message>
Added Undo Next Player feature
</commit_message>
<xml_diff>
--- a/players.xlsx
+++ b/players.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="274">
   <si>
     <t>Table 1</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>Pat Cummins</t>
+  </si>
+  <si>
+    <t>Jacob Duffy</t>
   </si>
   <si>
     <t>Anshul Kamboj</t>
@@ -1059,7 +1062,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1112,15 +1115,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2751,8 +2745,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="29" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="29" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="26" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -2787,7 +2781,7 @@
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B3" t="s" s="7">
         <v>8</v>
@@ -2807,7 +2801,7 @@
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="10">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B4" t="s" s="11">
         <v>8</v>
@@ -2827,7 +2821,7 @@
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="10">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s" s="11">
         <v>8</v>
@@ -2847,7 +2841,7 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="10">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B6" t="s" s="11">
         <v>15</v>
@@ -2867,7 +2861,7 @@
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="10">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B7" t="s" s="11">
         <v>15</v>
@@ -2887,7 +2881,7 @@
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="10">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B8" t="s" s="11">
         <v>15</v>
@@ -2907,7 +2901,7 @@
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="10">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B9" t="s" s="11">
         <v>15</v>
@@ -2927,7 +2921,7 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="10">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B10" t="s" s="11">
         <v>19</v>
@@ -2947,7 +2941,7 @@
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="10">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B11" t="s" s="11">
         <v>25</v>
@@ -2967,7 +2961,7 @@
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="10">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B12" t="s" s="11">
         <v>25</v>
@@ -2987,7 +2981,7 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="10">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B13" t="s" s="11">
         <v>25</v>
@@ -3007,7 +3001,7 @@
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="10">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B14" t="s" s="11">
         <v>25</v>
@@ -3027,7 +3021,7 @@
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="10">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B15" t="s" s="11">
         <v>36</v>
@@ -3047,7 +3041,7 @@
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="10">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B16" t="s" s="11">
         <v>36</v>
@@ -3067,7 +3061,7 @@
     </row>
     <row r="17" ht="32.05" customHeight="1">
       <c r="A17" t="s" s="10">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B17" t="s" s="11">
         <v>39</v>
@@ -3087,7 +3081,7 @@
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="10">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B18" t="s" s="11">
         <v>39</v>
@@ -3107,7 +3101,7 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="10">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B19" t="s" s="11">
         <v>42</v>
@@ -3127,7 +3121,7 @@
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="10">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B20" t="s" s="11">
         <v>45</v>
@@ -3147,7 +3141,7 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="10">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B21" t="s" s="11">
         <v>45</v>
@@ -3167,7 +3161,7 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="10">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B22" t="s" s="11">
         <v>45</v>
@@ -3187,7 +3181,7 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="10">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B23" t="s" s="11">
         <v>45</v>
@@ -4142,7 +4136,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.2031" style="16" customWidth="1"/>
+    <col min="1" max="1" width="18.1719" style="16" customWidth="1"/>
     <col min="2" max="6" width="16.3516" style="16" customWidth="1"/>
     <col min="7" max="16384" width="16.3516" style="16" customWidth="1"/>
   </cols>
@@ -4421,19 +4415,19 @@
       <c r="A15" t="s" s="17">
         <v>100</v>
       </c>
-      <c r="B15" t="s" s="18">
+      <c r="B15" t="s" s="11">
         <v>28</v>
       </c>
-      <c r="C15" t="s" s="19">
+      <c r="C15" t="s" s="12">
         <v>20</v>
       </c>
-      <c r="D15" t="s" s="19">
+      <c r="D15" t="s" s="12">
         <v>13</v>
       </c>
-      <c r="E15" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="F15" s="20">
+      <c r="E15" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="F15" s="13">
         <v>2</v>
       </c>
     </row>
@@ -4441,19 +4435,19 @@
       <c r="A16" t="s" s="17">
         <v>101</v>
       </c>
-      <c r="B16" t="s" s="18">
+      <c r="B16" t="s" s="11">
         <v>31</v>
       </c>
-      <c r="C16" t="s" s="19">
+      <c r="C16" t="s" s="12">
         <v>20</v>
       </c>
-      <c r="D16" t="s" s="19">
+      <c r="D16" t="s" s="12">
         <v>13</v>
       </c>
-      <c r="E16" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="F16" s="20">
+      <c r="E16" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="F16" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4483,7 +4477,7 @@
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="21"/>
+      <c r="F18" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4508,8 +4502,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="22" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -5039,14 +5033,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="23" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="23" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="20" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -5477,6 +5471,26 @@
       </c>
       <c r="F22" s="13">
         <v>2</v>
+      </c>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" t="s" s="10">
+        <v>147</v>
+      </c>
+      <c r="B23" t="s" s="11">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s" s="12">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s" s="12">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s" s="12">
+        <v>11</v>
+      </c>
+      <c r="F23" s="13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5502,8 +5516,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="24" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="24" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="21" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -5538,7 +5552,7 @@
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s" s="7">
         <v>8</v>
@@ -5550,7 +5564,7 @@
         <v>22</v>
       </c>
       <c r="E3" t="s" s="8">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F3" s="9">
         <v>0.5</v>
@@ -5558,7 +5572,7 @@
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="10">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B4" t="s" s="11">
         <v>8</v>
@@ -5570,7 +5584,7 @@
         <v>22</v>
       </c>
       <c r="E4" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F4" s="13">
         <v>0.5</v>
@@ -5578,7 +5592,7 @@
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="10">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s" s="11">
         <v>8</v>
@@ -5590,7 +5604,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F5" s="13">
         <v>0.5</v>
@@ -5598,7 +5612,7 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="10">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s" s="11">
         <v>8</v>
@@ -5610,7 +5624,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F6" s="13">
         <v>0.5</v>
@@ -5618,7 +5632,7 @@
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="10">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="11">
         <v>15</v>
@@ -5630,7 +5644,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F7" s="13">
         <v>0.5</v>
@@ -5638,7 +5652,7 @@
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="10">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s" s="11">
         <v>15</v>
@@ -5650,7 +5664,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F8" s="13">
         <v>0.5</v>
@@ -5658,7 +5672,7 @@
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="10">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s" s="11">
         <v>15</v>
@@ -5670,7 +5684,7 @@
         <v>16</v>
       </c>
       <c r="E9" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F9" s="13">
         <v>0.5</v>
@@ -5678,7 +5692,7 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="10">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s" s="11">
         <v>15</v>
@@ -5690,7 +5704,7 @@
         <v>22</v>
       </c>
       <c r="E10" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F10" s="13">
         <v>0.5</v>
@@ -5698,7 +5712,7 @@
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="10">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s" s="11">
         <v>19</v>
@@ -5710,7 +5724,7 @@
         <v>13</v>
       </c>
       <c r="E11" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F11" s="13">
         <v>1</v>
@@ -5718,7 +5732,7 @@
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="10">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s" s="11">
         <v>19</v>
@@ -5730,7 +5744,7 @@
         <v>13</v>
       </c>
       <c r="E12" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F12" s="13">
         <v>1</v>
@@ -5738,7 +5752,7 @@
     </row>
     <row r="13" ht="32.05" customHeight="1">
       <c r="A13" t="s" s="10">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s" s="11">
         <v>25</v>
@@ -5750,7 +5764,7 @@
         <v>13</v>
       </c>
       <c r="E13" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F13" s="13">
         <v>0.5</v>
@@ -5758,7 +5772,7 @@
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="10">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B14" t="s" s="11">
         <v>25</v>
@@ -5770,7 +5784,7 @@
         <v>22</v>
       </c>
       <c r="E14" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F14" s="13">
         <v>0.5</v>
@@ -5778,7 +5792,7 @@
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="10">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B15" t="s" s="11">
         <v>28</v>
@@ -5790,7 +5804,7 @@
         <v>16</v>
       </c>
       <c r="E15" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F15" s="13">
         <v>0.5</v>
@@ -5798,7 +5812,7 @@
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="10">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s" s="11">
         <v>28</v>
@@ -5810,7 +5824,7 @@
         <v>22</v>
       </c>
       <c r="E16" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F16" s="13">
         <v>0.5</v>
@@ -5818,7 +5832,7 @@
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="10">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B17" t="s" s="11">
         <v>31</v>
@@ -5830,7 +5844,7 @@
         <v>22</v>
       </c>
       <c r="E17" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F17" s="13">
         <v>0.5</v>
@@ -5838,7 +5852,7 @@
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="10">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s" s="11">
         <v>31</v>
@@ -5850,7 +5864,7 @@
         <v>16</v>
       </c>
       <c r="E18" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F18" s="13">
         <v>0.5</v>
@@ -5858,7 +5872,7 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="10">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s" s="11">
         <v>36</v>
@@ -5870,7 +5884,7 @@
         <v>16</v>
       </c>
       <c r="E19" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F19" s="13">
         <v>0.5</v>
@@ -5878,7 +5892,7 @@
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="10">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s" s="11">
         <v>36</v>
@@ -5890,7 +5904,7 @@
         <v>13</v>
       </c>
       <c r="E20" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F20" s="13">
         <v>0.5</v>
@@ -5898,7 +5912,7 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="10">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s" s="11">
         <v>36</v>
@@ -5910,7 +5924,7 @@
         <v>13</v>
       </c>
       <c r="E21" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F21" s="13">
         <v>0.5</v>
@@ -5918,7 +5932,7 @@
     </row>
     <row r="22" ht="32.05" customHeight="1">
       <c r="A22" t="s" s="10">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s" s="11">
         <v>36</v>
@@ -5930,7 +5944,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F22" s="13">
         <v>0.5</v>
@@ -5938,7 +5952,7 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="10">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s" s="11">
         <v>36</v>
@@ -5950,7 +5964,7 @@
         <v>13</v>
       </c>
       <c r="E23" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F23" s="13">
         <v>0.5</v>
@@ -5958,7 +5972,7 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="10">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B24" t="s" s="11">
         <v>36</v>
@@ -5970,7 +5984,7 @@
         <v>13</v>
       </c>
       <c r="E24" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F24" s="13">
         <v>1</v>
@@ -5978,7 +5992,7 @@
     </row>
     <row r="25" ht="32.05" customHeight="1">
       <c r="A25" t="s" s="10">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s" s="11">
         <v>39</v>
@@ -5990,7 +6004,7 @@
         <v>13</v>
       </c>
       <c r="E25" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F25" s="13">
         <v>1</v>
@@ -5998,7 +6012,7 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="10">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B26" t="s" s="11">
         <v>39</v>
@@ -6010,7 +6024,7 @@
         <v>22</v>
       </c>
       <c r="E26" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F26" s="13">
         <v>0.5</v>
@@ -6018,7 +6032,7 @@
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="10">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B27" t="s" s="11">
         <v>42</v>
@@ -6030,7 +6044,7 @@
         <v>22</v>
       </c>
       <c r="E27" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F27" s="13">
         <v>0.5</v>
@@ -6038,7 +6052,7 @@
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="10">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B28" t="s" s="11">
         <v>42</v>
@@ -6050,7 +6064,7 @@
         <v>22</v>
       </c>
       <c r="E28" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F28" s="13">
         <v>0.5</v>
@@ -6058,7 +6072,7 @@
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="10">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B29" t="s" s="11">
         <v>45</v>
@@ -6070,7 +6084,7 @@
         <v>22</v>
       </c>
       <c r="E29" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F29" s="13">
         <v>0.5</v>
@@ -6078,7 +6092,7 @@
     </row>
     <row r="30" ht="32.05" customHeight="1">
       <c r="A30" t="s" s="10">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B30" t="s" s="11">
         <v>45</v>
@@ -6090,7 +6104,7 @@
         <v>13</v>
       </c>
       <c r="E30" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F30" s="13">
         <v>0.5</v>
@@ -6119,8 +6133,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="25" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="25" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -6155,7 +6169,7 @@
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s" s="7">
         <v>8</v>
@@ -6167,7 +6181,7 @@
         <v>22</v>
       </c>
       <c r="E3" t="s" s="8">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F3" s="9">
         <v>0.5</v>
@@ -6175,7 +6189,7 @@
     </row>
     <row r="4" ht="32.05" customHeight="1">
       <c r="A4" t="s" s="10">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s" s="11">
         <v>8</v>
@@ -6187,7 +6201,7 @@
         <v>22</v>
       </c>
       <c r="E4" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F4" s="13">
         <v>0.5</v>
@@ -6195,7 +6209,7 @@
     </row>
     <row r="5" ht="32.05" customHeight="1">
       <c r="A5" t="s" s="10">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s" s="11">
         <v>8</v>
@@ -6207,7 +6221,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F5" s="13">
         <v>0.5</v>
@@ -6215,7 +6229,7 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="10">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s" s="11">
         <v>8</v>
@@ -6227,7 +6241,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F6" s="13">
         <v>0.5</v>
@@ -6235,7 +6249,7 @@
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="10">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s" s="11">
         <v>8</v>
@@ -6247,7 +6261,7 @@
         <v>16</v>
       </c>
       <c r="E7" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F7" s="13">
         <v>0.5</v>
@@ -6255,7 +6269,7 @@
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="10">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B8" t="s" s="11">
         <v>8</v>
@@ -6267,7 +6281,7 @@
         <v>16</v>
       </c>
       <c r="E8" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F8" s="13">
         <v>0.5</v>
@@ -6275,7 +6289,7 @@
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="10">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B9" t="s" s="11">
         <v>15</v>
@@ -6287,7 +6301,7 @@
         <v>13</v>
       </c>
       <c r="E9" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F9" s="13">
         <v>0.5</v>
@@ -6295,7 +6309,7 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="10">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B10" t="s" s="11">
         <v>15</v>
@@ -6307,7 +6321,7 @@
         <v>13</v>
       </c>
       <c r="E10" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F10" s="13">
         <v>0.5</v>
@@ -6315,7 +6329,7 @@
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="10">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B11" t="s" s="11">
         <v>15</v>
@@ -6327,7 +6341,7 @@
         <v>13</v>
       </c>
       <c r="E11" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F11" s="13">
         <v>0.5</v>
@@ -6335,7 +6349,7 @@
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="10">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B12" t="s" s="11">
         <v>15</v>
@@ -6347,7 +6361,7 @@
         <v>13</v>
       </c>
       <c r="E12" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F12" s="13">
         <v>0.5</v>
@@ -6355,7 +6369,7 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="10">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B13" t="s" s="11">
         <v>15</v>
@@ -6367,7 +6381,7 @@
         <v>16</v>
       </c>
       <c r="E13" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F13" s="13">
         <v>0.5</v>
@@ -6375,7 +6389,7 @@
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="10">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B14" t="s" s="11">
         <v>19</v>
@@ -6387,7 +6401,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F14" s="13">
         <v>0.5</v>
@@ -6395,7 +6409,7 @@
     </row>
     <row r="15" ht="32.05" customHeight="1">
       <c r="A15" t="s" s="10">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B15" t="s" s="11">
         <v>19</v>
@@ -6407,7 +6421,7 @@
         <v>22</v>
       </c>
       <c r="E15" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F15" s="13">
         <v>0.5</v>
@@ -6415,7 +6429,7 @@
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="10">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B16" t="s" s="11">
         <v>19</v>
@@ -6427,7 +6441,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F16" s="13">
         <v>0.5</v>
@@ -6435,7 +6449,7 @@
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="10">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s" s="11">
         <v>19</v>
@@ -6447,7 +6461,7 @@
         <v>22</v>
       </c>
       <c r="E17" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F17" s="13">
         <v>0.5</v>
@@ -6455,7 +6469,7 @@
     </row>
     <row r="18" ht="32.05" customHeight="1">
       <c r="A18" t="s" s="10">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s" s="11">
         <v>19</v>
@@ -6467,7 +6481,7 @@
         <v>16</v>
       </c>
       <c r="E18" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F18" s="13">
         <v>0.5</v>
@@ -6475,7 +6489,7 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="10">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B19" t="s" s="11">
         <v>19</v>
@@ -6487,7 +6501,7 @@
         <v>16</v>
       </c>
       <c r="E19" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F19" s="13">
         <v>0.5</v>
@@ -6495,7 +6509,7 @@
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="10">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B20" t="s" s="11">
         <v>19</v>
@@ -6507,7 +6521,7 @@
         <v>22</v>
       </c>
       <c r="E20" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F20" s="13">
         <v>0.5</v>
@@ -6515,7 +6529,7 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="10">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B21" t="s" s="11">
         <v>19</v>
@@ -6527,7 +6541,7 @@
         <v>22</v>
       </c>
       <c r="E21" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F21" s="13">
         <v>0.5</v>
@@ -6535,7 +6549,7 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="10">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B22" t="s" s="11">
         <v>25</v>
@@ -6547,7 +6561,7 @@
         <v>16</v>
       </c>
       <c r="E22" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F22" s="13">
         <v>0.5</v>
@@ -6555,7 +6569,7 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="10">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B23" t="s" s="11">
         <v>25</v>
@@ -6567,7 +6581,7 @@
         <v>10</v>
       </c>
       <c r="E23" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F23" s="13">
         <v>0.5</v>
@@ -6575,7 +6589,7 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="10">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B24" t="s" s="11">
         <v>25</v>
@@ -6587,7 +6601,7 @@
         <v>13</v>
       </c>
       <c r="E24" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F24" s="13">
         <v>0.5</v>
@@ -6595,7 +6609,7 @@
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="10">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B25" t="s" s="11">
         <v>25</v>
@@ -6607,7 +6621,7 @@
         <v>22</v>
       </c>
       <c r="E25" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F25" s="13">
         <v>0.5</v>
@@ -6615,7 +6629,7 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="10">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B26" t="s" s="11">
         <v>25</v>
@@ -6627,7 +6641,7 @@
         <v>22</v>
       </c>
       <c r="E26" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F26" s="13">
         <v>0.5</v>
@@ -6635,7 +6649,7 @@
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="10">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B27" t="s" s="11">
         <v>25</v>
@@ -6647,7 +6661,7 @@
         <v>22</v>
       </c>
       <c r="E27" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F27" s="13">
         <v>0.5</v>
@@ -6655,7 +6669,7 @@
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="10">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B28" t="s" s="11">
         <v>28</v>
@@ -6667,7 +6681,7 @@
         <v>13</v>
       </c>
       <c r="E28" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F28" s="13">
         <v>0.5</v>
@@ -6675,7 +6689,7 @@
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="10">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B29" t="s" s="11">
         <v>28</v>
@@ -6687,7 +6701,7 @@
         <v>22</v>
       </c>
       <c r="E29" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F29" s="13">
         <v>0.5</v>
@@ -6695,7 +6709,7 @@
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="10">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B30" t="s" s="11">
         <v>28</v>
@@ -6707,7 +6721,7 @@
         <v>16</v>
       </c>
       <c r="E30" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F30" s="13">
         <v>0.5</v>
@@ -6715,7 +6729,7 @@
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" t="s" s="10">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B31" t="s" s="11">
         <v>28</v>
@@ -6727,7 +6741,7 @@
         <v>13</v>
       </c>
       <c r="E31" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F31" s="13">
         <v>0.5</v>
@@ -6735,7 +6749,7 @@
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" t="s" s="10">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B32" t="s" s="11">
         <v>28</v>
@@ -6747,7 +6761,7 @@
         <v>16</v>
       </c>
       <c r="E32" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F32" s="13">
         <v>0.5</v>
@@ -6755,7 +6769,7 @@
     </row>
     <row r="33" ht="32.05" customHeight="1">
       <c r="A33" t="s" s="10">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B33" t="s" s="11">
         <v>28</v>
@@ -6767,7 +6781,7 @@
         <v>22</v>
       </c>
       <c r="E33" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F33" s="13">
         <v>0.5</v>
@@ -6775,7 +6789,7 @@
     </row>
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" t="s" s="10">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B34" t="s" s="11">
         <v>28</v>
@@ -6787,7 +6801,7 @@
         <v>22</v>
       </c>
       <c r="E34" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F34" s="13">
         <v>0.5</v>
@@ -6795,7 +6809,7 @@
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" t="s" s="10">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B35" t="s" s="11">
         <v>28</v>
@@ -6807,7 +6821,7 @@
         <v>22</v>
       </c>
       <c r="E35" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F35" s="13">
         <v>0.5</v>
@@ -6815,7 +6829,7 @@
     </row>
     <row r="36" ht="20.05" customHeight="1">
       <c r="A36" t="s" s="10">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B36" t="s" s="11">
         <v>28</v>
@@ -6827,7 +6841,7 @@
         <v>22</v>
       </c>
       <c r="E36" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F36" s="13">
         <v>0.5</v>
@@ -6835,7 +6849,7 @@
     </row>
     <row r="37" ht="32.05" customHeight="1">
       <c r="A37" t="s" s="10">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B37" t="s" s="11">
         <v>28</v>
@@ -6847,7 +6861,7 @@
         <v>13</v>
       </c>
       <c r="E37" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F37" s="13">
         <v>0.5</v>
@@ -6855,7 +6869,7 @@
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" t="s" s="10">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B38" t="s" s="11">
         <v>28</v>
@@ -6867,7 +6881,7 @@
         <v>22</v>
       </c>
       <c r="E38" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F38" s="13">
         <v>0.5</v>
@@ -6875,7 +6889,7 @@
     </row>
     <row r="39" ht="20.05" customHeight="1">
       <c r="A39" t="s" s="10">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B39" t="s" s="11">
         <v>31</v>
@@ -6887,7 +6901,7 @@
         <v>22</v>
       </c>
       <c r="E39" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F39" s="13">
         <v>0.5</v>
@@ -6895,7 +6909,7 @@
     </row>
     <row r="40" ht="20.05" customHeight="1">
       <c r="A40" t="s" s="10">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B40" t="s" s="11">
         <v>31</v>
@@ -6907,315 +6921,315 @@
         <v>16</v>
       </c>
       <c r="E40" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F40" s="13">
         <v>0.5</v>
       </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" s="26"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
+      <c r="A41" s="23"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
     </row>
     <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" s="26"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
+      <c r="A42" s="23"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
     </row>
     <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" s="26"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
     </row>
     <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
     </row>
     <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" s="26"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
     </row>
     <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" s="26"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
     </row>
     <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" s="26"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
     </row>
     <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" s="26"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
     </row>
     <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" s="26"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
     </row>
     <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" s="26"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
+      <c r="A50" s="23"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
     </row>
     <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" s="26"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
+      <c r="A51" s="23"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
     </row>
     <row r="52" ht="20.05" customHeight="1">
-      <c r="A52" s="26"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
+      <c r="A52" s="23"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
     </row>
     <row r="53" ht="20.05" customHeight="1">
-      <c r="A53" s="26"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
     </row>
     <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" s="26"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
+      <c r="A54" s="23"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
     </row>
     <row r="55" ht="20.05" customHeight="1">
-      <c r="A55" s="26"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
+      <c r="A55" s="23"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
     </row>
     <row r="56" ht="20.05" customHeight="1">
-      <c r="A56" s="26"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
+      <c r="A56" s="23"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
     </row>
     <row r="57" ht="20.05" customHeight="1">
-      <c r="A57" s="26"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
+      <c r="A57" s="23"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
     </row>
     <row r="58" ht="20.05" customHeight="1">
-      <c r="A58" s="26"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
     </row>
     <row r="59" ht="20.05" customHeight="1">
-      <c r="A59" s="26"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
     </row>
     <row r="60" ht="20.05" customHeight="1">
-      <c r="A60" s="26"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
     </row>
     <row r="61" ht="20.05" customHeight="1">
-      <c r="A61" s="26"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
     </row>
     <row r="62" ht="20.05" customHeight="1">
-      <c r="A62" s="26"/>
-      <c r="B62" s="27"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
     </row>
     <row r="63" ht="20.05" customHeight="1">
-      <c r="A63" s="26"/>
-      <c r="B63" s="27"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
+      <c r="A63" s="23"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
     </row>
     <row r="64" ht="20.05" customHeight="1">
-      <c r="A64" s="26"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
+      <c r="A64" s="23"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
     </row>
     <row r="65" ht="20.05" customHeight="1">
-      <c r="A65" s="26"/>
-      <c r="B65" s="27"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
+      <c r="A65" s="23"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
     </row>
     <row r="66" ht="20.05" customHeight="1">
-      <c r="A66" s="26"/>
-      <c r="B66" s="27"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
+      <c r="A66" s="23"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
     </row>
     <row r="67" ht="20.05" customHeight="1">
-      <c r="A67" s="26"/>
-      <c r="B67" s="27"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
+      <c r="A67" s="23"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+      <c r="F67" s="18"/>
     </row>
     <row r="68" ht="20.05" customHeight="1">
-      <c r="A68" s="26"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
+      <c r="A68" s="23"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
     </row>
     <row r="69" ht="20.05" customHeight="1">
-      <c r="A69" s="26"/>
-      <c r="B69" s="27"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
+      <c r="A69" s="23"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
     </row>
     <row r="70" ht="20.05" customHeight="1">
-      <c r="A70" s="26"/>
-      <c r="B70" s="27"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
+      <c r="A70" s="23"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
+      <c r="F70" s="18"/>
     </row>
     <row r="71" ht="20.05" customHeight="1">
-      <c r="A71" s="26"/>
-      <c r="B71" s="27"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
+      <c r="A71" s="23"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
     </row>
     <row r="72" ht="20.05" customHeight="1">
-      <c r="A72" s="26"/>
-      <c r="B72" s="27"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
+      <c r="A72" s="23"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
     </row>
     <row r="73" ht="20.05" customHeight="1">
-      <c r="A73" s="26"/>
-      <c r="B73" s="27"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
+      <c r="A73" s="23"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="18"/>
     </row>
     <row r="74" ht="20.05" customHeight="1">
-      <c r="A74" s="26"/>
-      <c r="B74" s="27"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
+      <c r="A74" s="23"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
     </row>
     <row r="75" ht="20.05" customHeight="1">
-      <c r="A75" s="26"/>
-      <c r="B75" s="27"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
+      <c r="A75" s="23"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
     </row>
     <row r="76" ht="20.05" customHeight="1">
-      <c r="A76" s="26"/>
-      <c r="B76" s="27"/>
-      <c r="C76" s="21"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="21"/>
-      <c r="F76" s="21"/>
+      <c r="A76" s="23"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
     </row>
     <row r="77" ht="20.05" customHeight="1">
-      <c r="A77" s="26"/>
-      <c r="B77" s="27"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="21"/>
-      <c r="F77" s="21"/>
+      <c r="A77" s="23"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
     </row>
     <row r="78" ht="20.05" customHeight="1">
-      <c r="A78" s="26"/>
-      <c r="B78" s="27"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
+      <c r="A78" s="23"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7240,8 +7254,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="28" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="28" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="25" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -7276,7 +7290,7 @@
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="6">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B3" t="s" s="7">
         <v>31</v>
@@ -7288,7 +7302,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s" s="8">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F3" s="9">
         <v>0.5</v>
@@ -7296,7 +7310,7 @@
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="10">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B4" t="s" s="11">
         <v>31</v>
@@ -7308,7 +7322,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F4" s="13">
         <v>0.5</v>
@@ -7316,7 +7330,7 @@
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="10">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B5" t="s" s="11">
         <v>31</v>
@@ -7328,7 +7342,7 @@
         <v>22</v>
       </c>
       <c r="E5" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F5" s="13">
         <v>0.5</v>
@@ -7336,7 +7350,7 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="10">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B6" t="s" s="11">
         <v>31</v>
@@ -7348,7 +7362,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F6" s="13">
         <v>0.5</v>
@@ -7356,7 +7370,7 @@
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="10">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B7" t="s" s="11">
         <v>31</v>
@@ -7368,7 +7382,7 @@
         <v>22</v>
       </c>
       <c r="E7" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F7" s="13">
         <v>0.5</v>
@@ -7376,7 +7390,7 @@
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="10">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B8" t="s" s="11">
         <v>36</v>
@@ -7388,7 +7402,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F8" s="13">
         <v>0.5</v>
@@ -7396,7 +7410,7 @@
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="10">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B9" t="s" s="11">
         <v>36</v>
@@ -7408,7 +7422,7 @@
         <v>13</v>
       </c>
       <c r="E9" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F9" s="13">
         <v>0.5</v>
@@ -7416,7 +7430,7 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="10">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s" s="11">
         <v>36</v>
@@ -7428,7 +7442,7 @@
         <v>16</v>
       </c>
       <c r="E10" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F10" s="13">
         <v>0.5</v>
@@ -7436,7 +7450,7 @@
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="10">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B11" t="s" s="11">
         <v>36</v>
@@ -7448,7 +7462,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F11" s="13">
         <v>0.5</v>
@@ -7456,7 +7470,7 @@
     </row>
     <row r="12" ht="32.05" customHeight="1">
       <c r="A12" t="s" s="10">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="11">
         <v>36</v>
@@ -7468,7 +7482,7 @@
         <v>22</v>
       </c>
       <c r="E12" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F12" s="13">
         <v>0.5</v>
@@ -7476,7 +7490,7 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="10">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B13" t="s" s="11">
         <v>36</v>
@@ -7488,7 +7502,7 @@
         <v>22</v>
       </c>
       <c r="E13" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F13" s="13">
         <v>0.5</v>
@@ -7496,7 +7510,7 @@
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="10">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s" s="11">
         <v>36</v>
@@ -7508,7 +7522,7 @@
         <v>22</v>
       </c>
       <c r="E14" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F14" s="13">
         <v>0.5</v>
@@ -7516,7 +7530,7 @@
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="10">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B15" t="s" s="11">
         <v>36</v>
@@ -7528,7 +7542,7 @@
         <v>22</v>
       </c>
       <c r="E15" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F15" s="13">
         <v>0.5</v>
@@ -7536,7 +7550,7 @@
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="10">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B16" t="s" s="11">
         <v>39</v>
@@ -7548,7 +7562,7 @@
         <v>13</v>
       </c>
       <c r="E16" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F16" s="13">
         <v>0.5</v>
@@ -7556,7 +7570,7 @@
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="10">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B17" t="s" s="11">
         <v>39</v>
@@ -7568,7 +7582,7 @@
         <v>22</v>
       </c>
       <c r="E17" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F17" s="13">
         <v>0.5</v>
@@ -7576,7 +7590,7 @@
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="10">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B18" t="s" s="11">
         <v>39</v>
@@ -7588,7 +7602,7 @@
         <v>16</v>
       </c>
       <c r="E18" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F18" s="13">
         <v>0.5</v>
@@ -7596,7 +7610,7 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="10">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B19" t="s" s="11">
         <v>39</v>
@@ -7608,7 +7622,7 @@
         <v>22</v>
       </c>
       <c r="E19" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F19" s="13">
         <v>0.5</v>
@@ -7616,7 +7630,7 @@
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="10">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B20" t="s" s="11">
         <v>39</v>
@@ -7628,7 +7642,7 @@
         <v>22</v>
       </c>
       <c r="E20" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F20" s="13">
         <v>0.5</v>
@@ -7636,7 +7650,7 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="10">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B21" t="s" s="11">
         <v>39</v>
@@ -7648,7 +7662,7 @@
         <v>16</v>
       </c>
       <c r="E21" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F21" s="13">
         <v>0.5</v>
@@ -7656,7 +7670,7 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="10">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B22" t="s" s="11">
         <v>39</v>
@@ -7668,7 +7682,7 @@
         <v>16</v>
       </c>
       <c r="E22" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F22" s="13">
         <v>0.5</v>
@@ -7676,7 +7690,7 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="10">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B23" t="s" s="11">
         <v>39</v>
@@ -7688,7 +7702,7 @@
         <v>16</v>
       </c>
       <c r="E23" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F23" s="13">
         <v>0.5</v>
@@ -7696,7 +7710,7 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="10">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B24" t="s" s="11">
         <v>42</v>
@@ -7708,7 +7722,7 @@
         <v>22</v>
       </c>
       <c r="E24" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F24" s="13">
         <v>0.5</v>
@@ -7716,7 +7730,7 @@
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="10">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B25" t="s" s="11">
         <v>42</v>
@@ -7728,7 +7742,7 @@
         <v>22</v>
       </c>
       <c r="E25" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F25" s="13">
         <v>0.5</v>
@@ -7736,7 +7750,7 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="10">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B26" t="s" s="11">
         <v>42</v>
@@ -7748,7 +7762,7 @@
         <v>16</v>
       </c>
       <c r="E26" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F26" s="13">
         <v>0.5</v>
@@ -7756,7 +7770,7 @@
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="10">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B27" t="s" s="11">
         <v>42</v>
@@ -7768,7 +7782,7 @@
         <v>22</v>
       </c>
       <c r="E27" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F27" s="13">
         <v>0.5</v>
@@ -7776,7 +7790,7 @@
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="10">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B28" t="s" s="11">
         <v>42</v>
@@ -7788,7 +7802,7 @@
         <v>16</v>
       </c>
       <c r="E28" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F28" s="13">
         <v>0.5</v>
@@ -7796,7 +7810,7 @@
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="10">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B29" t="s" s="11">
         <v>42</v>
@@ -7808,7 +7822,7 @@
         <v>13</v>
       </c>
       <c r="E29" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F29" s="13">
         <v>0.5</v>
@@ -7816,7 +7830,7 @@
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="10">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B30" t="s" s="11">
         <v>42</v>
@@ -7828,7 +7842,7 @@
         <v>22</v>
       </c>
       <c r="E30" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F30" s="13">
         <v>0.5</v>
@@ -7836,7 +7850,7 @@
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" t="s" s="10">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B31" t="s" s="11">
         <v>42</v>
@@ -7848,7 +7862,7 @@
         <v>16</v>
       </c>
       <c r="E31" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F31" s="13">
         <v>0.5</v>
@@ -7856,7 +7870,7 @@
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" t="s" s="10">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B32" t="s" s="11">
         <v>45</v>
@@ -7868,7 +7882,7 @@
         <v>13</v>
       </c>
       <c r="E32" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F32" s="13">
         <v>0.5</v>
@@ -7876,7 +7890,7 @@
     </row>
     <row r="33" ht="20.05" customHeight="1">
       <c r="A33" t="s" s="10">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B33" t="s" s="11">
         <v>45</v>
@@ -7888,7 +7902,7 @@
         <v>22</v>
       </c>
       <c r="E33" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F33" s="13">
         <v>0.5</v>
@@ -7896,7 +7910,7 @@
     </row>
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" t="s" s="10">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B34" t="s" s="11">
         <v>45</v>
@@ -7908,7 +7922,7 @@
         <v>10</v>
       </c>
       <c r="E34" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F34" s="13">
         <v>0.5</v>
@@ -7916,7 +7930,7 @@
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" t="s" s="10">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B35" t="s" s="11">
         <v>45</v>
@@ -7928,7 +7942,7 @@
         <v>16</v>
       </c>
       <c r="E35" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F35" s="13">
         <v>0.5</v>
@@ -7936,7 +7950,7 @@
     </row>
     <row r="36" ht="20.05" customHeight="1">
       <c r="A36" t="s" s="10">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B36" t="s" s="11">
         <v>45</v>
@@ -7948,7 +7962,7 @@
         <v>16</v>
       </c>
       <c r="E36" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F36" s="13">
         <v>0.5</v>
@@ -7956,7 +7970,7 @@
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" t="s" s="10">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B37" t="s" s="11">
         <v>45</v>
@@ -7968,7 +7982,7 @@
         <v>22</v>
       </c>
       <c r="E37" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F37" s="13">
         <v>0.5</v>
@@ -7976,7 +7990,7 @@
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" t="s" s="10">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B38" t="s" s="11">
         <v>45</v>
@@ -7988,7 +8002,7 @@
         <v>22</v>
       </c>
       <c r="E38" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F38" s="13">
         <v>0.5</v>
@@ -7996,7 +8010,7 @@
     </row>
     <row r="39" ht="20.05" customHeight="1">
       <c r="A39" t="s" s="10">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B39" t="s" s="11">
         <v>45</v>
@@ -8008,7 +8022,7 @@
         <v>16</v>
       </c>
       <c r="E39" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F39" s="13">
         <v>0.5</v>
@@ -8016,7 +8030,7 @@
     </row>
     <row r="40" ht="20.05" customHeight="1">
       <c r="A40" t="s" s="10">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B40" t="s" s="11">
         <v>45</v>
@@ -8028,7 +8042,7 @@
         <v>16</v>
       </c>
       <c r="E40" t="s" s="12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F40" s="13">
         <v>0.5</v>

</xml_diff>